<commit_message>
Update value_set_list_with_code_count_version.xlsx to align
</commit_message>
<xml_diff>
--- a/codevalidator-api/docs/value_set_list_with_code_count_version.xlsx
+++ b/codevalidator-api/docs/value_set_list_with_code_count_version.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sneha Thalluri\Desktop\value sets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sneha Thalluri\Desktop\Agile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="254">
   <si>
     <t>Name</t>
   </si>
@@ -474,9 +474,6 @@
     <t>urn:oid:2.16.840.1.113883.11.20.9.37</t>
   </si>
   <si>
-    <t>Telecom Use (US Realm Header)</t>
-  </si>
-  <si>
     <t>urn:oid:2.16.840.1.113883.11.20.9.20</t>
   </si>
   <si>
@@ -517,9 +514,6 @@
   </si>
   <si>
     <t>urn:oid:2.16.840.1.113883.1.11.20.2.6</t>
-  </si>
-  <si>
-    <t>x_ServiceEventPerformer</t>
   </si>
   <si>
     <t>urn:oid:2.16.840.1.113883.1.11.19601</t>
@@ -598,9 +592,6 @@
     <t>http://www.census.gov/geo/reference/ansi_statetables.html</t>
   </si>
   <si>
-    <t>Substance-Reactant for Intolerance</t>
-  </si>
-  <si>
     <t>urn:oid:2.16.840.1.113762.1.4.1010.1</t>
   </si>
   <si>
@@ -659,9 +650,6 @@
 Substance Other Than Clinical Drug (2.16.840.1.113762.1.4.1010.9):(https://vsac.nlm.nih.gov/valuesets) </t>
   </si>
   <si>
-    <t>Substance Other Than Clinical Drug</t>
-  </si>
-  <si>
     <t>urn:oid:2.16.840.1.113762.1.4.1010.9</t>
   </si>
   <si>
@@ -792,6 +780,24 @@
   </si>
   <si>
     <t>urn:oid:2.16.840.1.113883.11.20.7.1</t>
+  </si>
+  <si>
+    <t>DIRDocumentTypeCodes</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.11.20.9.32</t>
+  </si>
+  <si>
+    <t>XServiceEventPerformer</t>
+  </si>
+  <si>
+    <t>TelecomUseUSRealmHeader</t>
+  </si>
+  <si>
+    <t>SubstanceReactantForIntolerance</t>
+  </si>
+  <si>
+    <t>SubstanceOtherThanClinical Drug</t>
   </si>
 </sst>
 </file>
@@ -922,7 +928,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1011,6 +1017,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1404,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106"/>
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,19 +1446,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1474,7 +1486,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>79</v>
@@ -1520,10 +1532,10 @@
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C5" s="8">
         <v>10</v>
@@ -1532,16 +1544,16 @@
         <v>10</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F5" s="15">
         <v>20130801</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1584,7 +1596,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G7" s="11">
         <v>20161010</v>
@@ -1607,7 +1619,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G8" s="11">
         <v>20150424</v>
@@ -1630,7 +1642,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G9" s="11">
         <v>20150528</v>
@@ -1638,33 +1650,33 @@
     </row>
     <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6</v>
+      </c>
+      <c r="D10" s="8">
+        <v>6</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C10" s="8">
-        <v>6</v>
-      </c>
-      <c r="D10" s="8">
-        <v>6</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>169</v>
-      </c>
       <c r="F10" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>17</v>
@@ -1679,7 +1691,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G11" s="11">
         <v>20150424</v>
@@ -1702,7 +1714,7 @@
         <v>6</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G12" s="11">
         <v>20160623</v>
@@ -1725,7 +1737,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G13" s="11">
         <v>20160903</v>
@@ -1733,10 +1745,10 @@
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C14" s="8">
         <v>24074</v>
@@ -1748,7 +1760,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G14" s="15">
         <v>20170601</v>
@@ -1771,7 +1783,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G15" s="11">
         <v>20150424</v>
@@ -1780,10 +1792,10 @@
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C16" s="8">
         <v>249</v>
@@ -1792,13 +1804,13 @@
         <v>249</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1818,7 +1830,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G17" s="11">
         <v>20150424</v>
@@ -1826,10 +1838,10 @@
     </row>
     <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C18" s="18">
         <v>3</v>
@@ -1841,7 +1853,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G18" s="15">
         <v>20170915</v>
@@ -1850,7 +1862,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>26</v>
@@ -1865,7 +1877,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G19" s="11">
         <v>20150819</v>
@@ -1888,10 +1900,10 @@
         <v>6</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1934,7 +1946,7 @@
         <v>6</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G22" s="11">
         <v>20150424</v>
@@ -1957,7 +1969,7 @@
         <v>6</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G23" s="11">
         <v>20150424</v>
@@ -1980,7 +1992,7 @@
         <v>6</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G24" s="11">
         <v>20160903</v>
@@ -2049,7 +2061,7 @@
         <v>6</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G27" s="11">
         <v>20150310</v>
@@ -2072,7 +2084,7 @@
         <v>6</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G28" s="11">
         <v>20121025</v>
@@ -2095,7 +2107,7 @@
         <v>6</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G29" s="11">
         <v>20150424</v>
@@ -2118,7 +2130,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G30" s="11">
         <v>20170106</v>
@@ -2149,10 +2161,10 @@
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C32" s="8">
         <v>848</v>
@@ -2161,10 +2173,10 @@
         <v>853</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="G32" s="11">
         <v>20170621</v>
@@ -2187,7 +2199,7 @@
         <v>6</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G33" s="11">
         <v>20150424</v>
@@ -2210,7 +2222,7 @@
         <v>6</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G34" s="11">
         <v>20170304</v>
@@ -2233,7 +2245,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G35" s="11">
         <v>20150310</v>
@@ -2241,7 +2253,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>57</v>
@@ -2256,7 +2268,7 @@
         <v>6</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G36" s="11">
         <v>20150424</v>
@@ -2279,7 +2291,7 @@
         <v>6</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G37" s="11">
         <v>20150424</v>
@@ -2302,7 +2314,7 @@
         <v>6</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G38" s="11">
         <v>20150310</v>
@@ -2310,10 +2322,10 @@
     </row>
     <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C39" s="8">
         <v>7982</v>
@@ -2322,13 +2334,13 @@
         <v>7982</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2371,7 +2383,7 @@
         <v>6</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G41" s="11">
         <v>20150424</v>
@@ -2394,7 +2406,7 @@
         <v>6</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G42" s="11">
         <v>20160903</v>
@@ -2417,7 +2429,7 @@
         <v>6</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G43" s="11">
         <v>20150424</v>
@@ -2425,10 +2437,10 @@
     </row>
     <row r="44" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C44" s="8">
         <v>64742</v>
@@ -2437,16 +2449,16 @@
         <v>88451</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G44" s="11">
         <v>20170601</v>
       </c>
       <c r="H44" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -2466,7 +2478,7 @@
         <v>6</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G45" s="11">
         <v>20150424</v>
@@ -2474,7 +2486,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>72</v>
@@ -2535,7 +2547,7 @@
         <v>6</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G48" s="11">
         <v>20161104</v>
@@ -2558,7 +2570,7 @@
         <v>6</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G49" s="11">
         <v>20150310</v>
@@ -2581,7 +2593,7 @@
         <v>6</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G50" s="11">
         <v>20161104</v>
@@ -2696,7 +2708,7 @@
         <v>6</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G55" s="15">
         <v>20161104</v>
@@ -2719,7 +2731,7 @@
         <v>6</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G56" s="11">
         <v>20161108</v>
@@ -2742,7 +2754,7 @@
         <v>6</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G57" s="11">
         <v>20161112</v>
@@ -2765,7 +2777,7 @@
         <v>6</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G58" s="11">
         <v>20161104</v>
@@ -2788,7 +2800,7 @@
         <v>6</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G59" s="11">
         <v>20161104</v>
@@ -2796,7 +2808,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>100</v>
@@ -2819,7 +2831,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>101</v>
@@ -2834,7 +2846,7 @@
         <v>6</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G61" s="11">
         <v>20150417</v>
@@ -2842,7 +2854,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>102</v>
@@ -2857,7 +2869,7 @@
         <v>6</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G62" s="11">
         <v>20150417</v>
@@ -2880,7 +2892,7 @@
         <v>6</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G63" s="11">
         <v>20150417</v>
@@ -2888,10 +2900,10 @@
     </row>
     <row r="64" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C64" s="8">
         <v>41440</v>
@@ -2900,13 +2912,13 @@
         <v>41440</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2926,7 +2938,7 @@
         <v>6</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G65" s="11">
         <v>20150424</v>
@@ -2949,7 +2961,7 @@
         <v>6</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G66" s="11">
         <v>20150424</v>
@@ -2972,7 +2984,7 @@
         <v>6</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G67" s="11">
         <v>20160712</v>
@@ -2995,7 +3007,7 @@
         <v>6</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G68" s="11">
         <v>20170504</v>
@@ -3018,7 +3030,7 @@
         <v>6</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G69" s="11">
         <v>20150424</v>
@@ -3026,7 +3038,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>115</v>
@@ -3041,7 +3053,7 @@
         <v>6</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G70" s="11">
         <v>20150424</v>
@@ -3064,7 +3076,7 @@
         <v>6</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G71" s="11">
         <v>20150826</v>
@@ -3087,7 +3099,7 @@
         <v>6</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G72" s="11">
         <v>20150819</v>
@@ -3110,7 +3122,7 @@
         <v>6</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G73" s="11">
         <v>20150424</v>
@@ -3133,7 +3145,7 @@
         <v>6</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G74" s="11">
         <v>20150424</v>
@@ -3156,7 +3168,7 @@
         <v>6</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G75" s="11">
         <v>20150424</v>
@@ -3179,7 +3191,7 @@
         <v>6</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G76" s="11">
         <v>20150424</v>
@@ -3225,7 +3237,7 @@
         <v>6</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G78" s="11">
         <v>20161112</v>
@@ -3248,7 +3260,7 @@
         <v>6</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G79" s="11">
         <v>20161104</v>
@@ -3271,7 +3283,7 @@
         <v>6</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G80" s="11">
         <v>20170426</v>
@@ -3294,7 +3306,7 @@
         <v>6</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G81" s="11">
         <v>20150424</v>
@@ -3317,7 +3329,7 @@
         <v>6</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G82" s="11">
         <v>20160712</v>
@@ -3340,7 +3352,7 @@
         <v>6</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G83" s="11">
         <v>20150407</v>
@@ -3348,7 +3360,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>142</v>
@@ -3363,7 +3375,7 @@
         <v>6</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G84" s="11">
         <v>20160712</v>
@@ -3371,7 +3383,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>143</v>
@@ -3386,7 +3398,7 @@
         <v>6</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G85" s="11">
         <v>20150407</v>
@@ -3394,10 +3406,10 @@
     </row>
     <row r="86" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C86" s="8">
         <v>51</v>
@@ -3406,21 +3418,21 @@
         <v>51</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G86" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="12" t="s">
-        <v>207</v>
+      <c r="A87" s="25" t="s">
+        <v>253</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C87" s="8">
         <v>4803</v>
@@ -3432,18 +3444,18 @@
         <v>6</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G87" s="11">
         <v>20170520</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A88" s="20" t="s">
-        <v>188</v>
+      <c r="A88" s="34" t="s">
+        <v>252</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C88" s="8">
         <v>732086</v>
@@ -3452,16 +3464,16 @@
         <v>57534</v>
       </c>
       <c r="E88" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F88" s="13" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G88" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H88" s="23" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -3481,7 +3493,7 @@
         <v>6</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G89" s="11">
         <v>20150424</v>
@@ -3504,7 +3516,7 @@
         <v>6</v>
       </c>
       <c r="F90" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G90" s="11">
         <v>20150424</v>
@@ -3512,10 +3524,10 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B91" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="C91" s="8">
         <v>4</v>
@@ -3527,7 +3539,7 @@
         <v>6</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G91" s="11">
         <v>20150424</v>
@@ -3535,10 +3547,10 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>151</v>
       </c>
       <c r="C92" s="8">
         <v>100</v>
@@ -3558,10 +3570,10 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>152</v>
-      </c>
-      <c r="B93" s="7" t="s">
-        <v>153</v>
       </c>
       <c r="C93" s="8">
         <v>60</v>
@@ -3581,10 +3593,10 @@
     </row>
     <row r="94" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C94" s="8">
         <v>813</v>
@@ -3593,24 +3605,24 @@
         <v>810</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="G94" s="16" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H94" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B95" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>155</v>
       </c>
       <c r="C95" s="8">
         <v>293</v>
@@ -3622,7 +3634,7 @@
         <v>6</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G95" s="11">
         <v>20161129</v>
@@ -3630,10 +3642,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C96" s="8">
         <v>11</v>
@@ -3645,7 +3657,7 @@
         <v>6</v>
       </c>
       <c r="F96" s="19" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G96" s="15">
         <v>20150424</v>
@@ -3653,10 +3665,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B97" s="7" t="s">
         <v>157</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="C97" s="8">
         <v>12</v>
@@ -3668,7 +3680,7 @@
         <v>6</v>
       </c>
       <c r="F97" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G97" s="11">
         <v>20160712</v>
@@ -3676,10 +3688,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B98" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="C98" s="8">
         <v>3</v>
@@ -3691,7 +3703,7 @@
         <v>6</v>
       </c>
       <c r="F98" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G98" s="11">
         <v>20160712</v>
@@ -3699,10 +3711,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>162</v>
       </c>
       <c r="C99" s="8">
         <v>14</v>
@@ -3714,18 +3726,18 @@
         <v>6</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G99" s="11">
         <v>20160712</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A100" s="12" t="s">
-        <v>163</v>
+      <c r="A100" s="25" t="s">
+        <v>250</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C100" s="8">
         <v>3</v>
@@ -3737,7 +3749,7 @@
         <v>6</v>
       </c>
       <c r="F100" s="19" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G100" s="11">
         <v>20170426</v>
@@ -3745,13 +3757,13 @@
     </row>
     <row r="101" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="27" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C101" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D101" s="29">
         <v>108582</v>
@@ -3760,7 +3772,7 @@
         <v>6</v>
       </c>
       <c r="F101" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G101" s="15">
         <v>20180122</v>
@@ -3768,13 +3780,13 @@
     </row>
     <row r="102" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B102" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C102" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D102" s="24">
         <v>29830</v>
@@ -3783,7 +3795,7 @@
         <v>6</v>
       </c>
       <c r="F102" s="30" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G102" s="31">
         <v>20160623</v>
@@ -3791,10 +3803,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B103" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C103" s="8">
         <v>9</v>
@@ -3806,11 +3818,41 @@
         <v>6</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G103" s="32">
         <v>20180112</v>
       </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B104" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="C104" s="8">
+        <v>5</v>
+      </c>
+      <c r="D104" s="8">
+        <v>5</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F104" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="G104" s="33" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="33"/>
+      <c r="B105" s="33"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="33"/>
+      <c r="G105" s="33"/>
     </row>
   </sheetData>
   <sortState ref="A2:G100">

</xml_diff>